<commit_message>
Add approve request functionality with associated variables and keywords
</commit_message>
<xml_diff>
--- a/ProjectTest65/Excel/EditIncomeAndExpense.xlsx
+++ b/ProjectTest65/Excel/EditIncomeAndExpense.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\acer\Desktop\Project\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\MiniProjectTest\ProjectTest65\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8046BC4-EB35-48AF-BDE8-02D7A4FE65E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E1DFBB-0F7E-4484-BFEC-7190F9BA2288}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{22BA047D-723E-4B76-82C5-5086CEEFFCA5}"/>
+    <workbookView xWindow="3060" yWindow="1908" windowWidth="17280" windowHeight="8112" xr2:uid="{22BA047D-723E-4B76-82C5-5086CEEFFCA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -459,7 +459,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="I8" sqref="I8:J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>

</xml_diff>